<commit_message>
Edition: I added all the comments in driver class in arduino firmware version 1.0.0.0
</commit_message>
<xml_diff>
--- a/Cost/Multi Size opration.xlsx
+++ b/Cost/Multi Size opration.xlsx
@@ -196,7 +196,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;Rs&quot;_ ;_ * \(#,##0.00\)\ &quot;Rs&quot;_ ;_ * &quot;-&quot;??_)\ &quot;Rs&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Rs&quot;"/>
-    <numFmt numFmtId="171" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -696,56 +696,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -753,9 +708,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -763,19 +715,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -791,6 +734,63 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:Y135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,9 +1097,9 @@
     <col min="14" max="14" width="17.109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" style="1"/>
     <col min="16" max="16" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.77734375" style="73" customWidth="1"/>
+    <col min="17" max="17" width="32.77734375" style="57" customWidth="1"/>
     <col min="18" max="18" width="51.5546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="72" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="56" customWidth="1"/>
     <col min="20" max="20" width="17.109375" style="10" customWidth="1"/>
     <col min="21" max="21" width="19.44140625" style="10" customWidth="1"/>
     <col min="22" max="22" width="20.33203125" style="10" customWidth="1"/>
@@ -1112,26 +1112,26 @@
     <row r="4" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="3:25" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="D5" s="2"/>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54"/>
-      <c r="K5" s="63" t="s">
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="79"/>
+      <c r="K5" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="65"/>
-      <c r="Q5" s="75" t="s">
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="71"/>
+      <c r="Q5" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="76"/>
-      <c r="U5" s="76"/>
-      <c r="V5" s="77"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="68"/>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="59"/>
     </row>
     <row r="6" spans="3:25" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -1147,7 +1147,7 @@
       <c r="H6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -1159,22 +1159,22 @@
       <c r="N6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="78" t="s">
+      <c r="Q6" s="60" t="s">
         <v>41</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S6" s="74" t="s">
+      <c r="S6" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="62" t="s">
+      <c r="T6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="62" t="s">
+      <c r="U6" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="V6" s="68" t="s">
+      <c r="V6" s="53" t="s">
         <v>53</v>
       </c>
       <c r="X6" s="4" t="s">
@@ -1206,7 +1206,7 @@
         <f>L7*M7</f>
         <v>30400</v>
       </c>
-      <c r="Q7" s="79">
+      <c r="Q7" s="72">
         <v>44423</v>
       </c>
       <c r="R7" s="6" t="s">
@@ -1230,7 +1230,7 @@
       <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="82" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -1247,7 +1247,7 @@
         <v>5070</v>
       </c>
       <c r="J8" s="44"/>
-      <c r="K8" s="67" t="s">
+      <c r="K8" s="52" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="7">
@@ -1261,7 +1261,7 @@
         <f>L8*M8</f>
         <v>4720</v>
       </c>
-      <c r="Q8" s="79"/>
+      <c r="Q8" s="72"/>
       <c r="R8" s="6" t="s">
         <v>46</v>
       </c>
@@ -1285,10 +1285,10 @@
       </c>
     </row>
     <row r="9" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="76"/>
       <c r="E9" s="11" t="s">
         <v>9</v>
       </c>
@@ -1311,13 +1311,13 @@
       </c>
       <c r="M9" s="8">
         <f>H36</f>
-        <v>22880</v>
+        <v>13690</v>
       </c>
       <c r="N9" s="9">
         <f>L9*M9</f>
-        <v>22880</v>
-      </c>
-      <c r="Q9" s="79"/>
+        <v>13690</v>
+      </c>
+      <c r="Q9" s="72"/>
       <c r="R9" s="6" t="s">
         <v>47</v>
       </c>
@@ -1328,14 +1328,14 @@
         <v>175</v>
       </c>
       <c r="U9" s="15">
-        <f t="shared" ref="U9:U33" si="1">S9*T9</f>
+        <f t="shared" ref="U9:U12" si="1">S9*T9</f>
         <v>350</v>
       </c>
       <c r="V9" s="9"/>
     </row>
     <row r="10" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C10" s="59"/>
-      <c r="D10" s="51"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="76"/>
       <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>1320</v>
       </c>
       <c r="J10" s="30"/>
-      <c r="K10" s="67" t="s">
+      <c r="K10" s="52" t="s">
         <v>37</v>
       </c>
       <c r="L10" s="7">
@@ -1364,7 +1364,7 @@
         <f>L10*M10</f>
         <v>2935</v>
       </c>
-      <c r="Q10" s="79"/>
+      <c r="Q10" s="72"/>
       <c r="R10" s="6" t="s">
         <v>48</v>
       </c>
@@ -1381,10 +1381,10 @@
       <c r="V10" s="9"/>
     </row>
     <row r="11" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="76"/>
       <c r="E11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1403,8 +1403,8 @@
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="Q11" s="80"/>
-      <c r="R11" s="85" t="s">
+      <c r="Q11" s="61"/>
+      <c r="R11" s="66" t="s">
         <v>54</v>
       </c>
       <c r="S11" s="7">
@@ -1420,10 +1420,10 @@
       <c r="V11" s="9"/>
     </row>
     <row r="12" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="76"/>
       <c r="E12" s="11" t="s">
         <v>6</v>
       </c>
@@ -1438,11 +1438,11 @@
         <v>1420</v>
       </c>
       <c r="J12" s="30"/>
-      <c r="K12" s="67"/>
+      <c r="K12" s="52"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="Q12" s="80"/>
+      <c r="Q12" s="61"/>
       <c r="R12" s="6" t="s">
         <v>55</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="V12" s="9"/>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="D13" s="51"/>
+      <c r="D13" s="76"/>
       <c r="E13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1474,16 +1474,16 @@
         <v>2000</v>
       </c>
       <c r="J13" s="30"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="61" t="s">
+      <c r="K13" s="52"/>
+      <c r="L13" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="61"/>
-      <c r="N13" s="68">
+      <c r="M13" s="81"/>
+      <c r="N13" s="53">
         <f>SUM(N7:N10)</f>
-        <v>60935</v>
-      </c>
-      <c r="Q13" s="80"/>
+        <v>51745</v>
+      </c>
+      <c r="Q13" s="61"/>
       <c r="R13" s="6"/>
       <c r="S13" s="7"/>
       <c r="T13" s="15"/>
@@ -1491,10 +1491,10 @@
       <c r="V13" s="9"/>
     </row>
     <row r="14" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="51"/>
+      <c r="D14" s="76"/>
       <c r="E14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1509,16 +1509,16 @@
         <v>280</v>
       </c>
       <c r="J14" s="30"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="70" t="s">
+      <c r="K14" s="54"/>
+      <c r="L14" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="70"/>
-      <c r="N14" s="71">
+      <c r="M14" s="80"/>
+      <c r="N14" s="55">
         <f>115000-N13</f>
-        <v>54065</v>
-      </c>
-      <c r="Q14" s="80"/>
+        <v>63255</v>
+      </c>
+      <c r="Q14" s="61"/>
       <c r="R14" s="6"/>
       <c r="S14" s="7"/>
       <c r="T14" s="15"/>
@@ -1526,10 +1526,10 @@
       <c r="V14" s="9"/>
     </row>
     <row r="15" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1548,7 +1548,7 @@
       <c r="L15" s="31"/>
       <c r="M15" s="14"/>
       <c r="N15" s="32"/>
-      <c r="Q15" s="80"/>
+      <c r="Q15" s="61"/>
       <c r="R15" s="6"/>
       <c r="S15" s="7"/>
       <c r="T15" s="15"/>
@@ -1556,10 +1556,10 @@
       <c r="V15" s="9"/>
     </row>
     <row r="16" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="51"/>
+      <c r="D16" s="76"/>
       <c r="E16" s="11" t="s">
         <v>13</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="L16" s="31"/>
       <c r="M16" s="14"/>
       <c r="N16" s="32"/>
-      <c r="Q16" s="80"/>
+      <c r="Q16" s="61"/>
       <c r="R16" s="6"/>
       <c r="S16" s="7"/>
       <c r="T16" s="15"/>
@@ -1586,10 +1586,10 @@
       <c r="V16" s="9"/>
     </row>
     <row r="17" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="52"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
@@ -1608,7 +1608,7 @@
       <c r="L17" s="31"/>
       <c r="M17" s="14"/>
       <c r="N17" s="32"/>
-      <c r="Q17" s="80"/>
+      <c r="Q17" s="61"/>
       <c r="R17" s="6"/>
       <c r="S17" s="7"/>
       <c r="T17" s="15"/>
@@ -1618,10 +1618,10 @@
     <row r="18" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="23"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="49"/>
+      <c r="G18" s="74"/>
       <c r="H18" s="25">
         <f>SUM(H8:H17)</f>
         <v>15200</v>
@@ -1631,7 +1631,7 @@
       <c r="L18" s="31"/>
       <c r="M18" s="14"/>
       <c r="N18" s="32"/>
-      <c r="Q18" s="80"/>
+      <c r="Q18" s="61"/>
       <c r="R18" s="6"/>
       <c r="S18" s="7"/>
       <c r="T18" s="15"/>
@@ -1645,14 +1645,14 @@
       <c r="G19" s="36"/>
       <c r="H19" s="37"/>
       <c r="J19" s="30"/>
-      <c r="K19" s="85">
+      <c r="K19" s="66">
         <f>H18-H13+1890+H21+H22+H25+H39+SUM(H41:H43)-H10-H17</f>
         <v>18095</v>
       </c>
       <c r="L19" s="31"/>
       <c r="M19" s="14"/>
       <c r="N19" s="32"/>
-      <c r="Q19" s="80"/>
+      <c r="Q19" s="61"/>
       <c r="R19" s="6"/>
       <c r="S19" s="7"/>
       <c r="T19" s="15"/>
@@ -1665,12 +1665,12 @@
       <c r="F20" s="40"/>
       <c r="G20" s="41"/>
       <c r="H20" s="42"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="Q20" s="80"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="Q20" s="61"/>
       <c r="R20" s="6"/>
       <c r="S20" s="7"/>
       <c r="T20" s="15"/>
@@ -1678,10 +1678,10 @@
       <c r="V20" s="9"/>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="76" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="26" t="s">
@@ -1702,7 +1702,7 @@
       <c r="L21" s="31"/>
       <c r="M21" s="14"/>
       <c r="N21" s="32"/>
-      <c r="Q21" s="80"/>
+      <c r="Q21" s="61"/>
       <c r="R21" s="6"/>
       <c r="S21" s="7"/>
       <c r="T21" s="15"/>
@@ -1710,7 +1710,7 @@
       <c r="V21" s="9"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D22" s="51"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="12" t="s">
         <v>19</v>
       </c>
@@ -1729,7 +1729,7 @@
       <c r="L22" s="31"/>
       <c r="M22" s="14"/>
       <c r="N22" s="32"/>
-      <c r="Q22" s="80"/>
+      <c r="Q22" s="61"/>
       <c r="R22" s="6"/>
       <c r="S22" s="7"/>
       <c r="T22" s="15"/>
@@ -1737,7 +1737,7 @@
       <c r="V22" s="9"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D23" s="51"/>
+      <c r="D23" s="76"/>
       <c r="E23" s="11" t="s">
         <v>20</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="L23" s="31"/>
       <c r="M23" s="14"/>
       <c r="N23" s="32"/>
-      <c r="Q23" s="80"/>
+      <c r="Q23" s="61"/>
       <c r="R23" s="6"/>
       <c r="S23" s="7"/>
       <c r="T23" s="15"/>
@@ -1764,7 +1764,7 @@
       <c r="V23" s="9"/>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D24" s="51"/>
+      <c r="D24" s="76"/>
       <c r="E24" s="6" t="s">
         <v>18</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="L24" s="31"/>
       <c r="M24" s="14"/>
       <c r="N24" s="32"/>
-      <c r="Q24" s="80"/>
+      <c r="Q24" s="61"/>
       <c r="R24" s="6"/>
       <c r="S24" s="7"/>
       <c r="T24" s="15"/>
@@ -1791,7 +1791,7 @@
       <c r="V24" s="9"/>
     </row>
     <row r="25" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D25" s="52"/>
+      <c r="D25" s="77"/>
       <c r="E25" s="12" t="s">
         <v>15</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="L25" s="31"/>
       <c r="M25" s="14"/>
       <c r="N25" s="32"/>
-      <c r="Q25" s="80"/>
+      <c r="Q25" s="61"/>
       <c r="R25" s="6"/>
       <c r="S25" s="7"/>
       <c r="T25" s="15"/>
@@ -1820,10 +1820,10 @@
     <row r="26" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="23"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="49"/>
+      <c r="G26" s="74"/>
       <c r="H26" s="25">
         <f>SUM(H21:H25)</f>
         <v>4720</v>
@@ -1833,7 +1833,7 @@
       <c r="L26" s="31"/>
       <c r="M26" s="14"/>
       <c r="N26" s="32"/>
-      <c r="Q26" s="80"/>
+      <c r="Q26" s="61"/>
       <c r="R26" s="6"/>
       <c r="S26" s="7"/>
       <c r="T26" s="15"/>
@@ -1851,7 +1851,7 @@
       <c r="L27" s="31"/>
       <c r="M27" s="14"/>
       <c r="N27" s="32"/>
-      <c r="Q27" s="80"/>
+      <c r="Q27" s="61"/>
       <c r="R27" s="6"/>
       <c r="S27" s="7"/>
       <c r="T27" s="15"/>
@@ -1869,7 +1869,7 @@
       <c r="L28" s="44"/>
       <c r="M28" s="32"/>
       <c r="N28" s="32"/>
-      <c r="Q28" s="80"/>
+      <c r="Q28" s="61"/>
       <c r="R28" s="6"/>
       <c r="S28" s="7"/>
       <c r="T28" s="15"/>
@@ -1877,7 +1877,7 @@
       <c r="V28" s="9"/>
     </row>
     <row r="29" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D29" s="56" t="s">
+      <c r="D29" s="83" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="26" t="s">
@@ -1887,18 +1887,18 @@
         <v>1</v>
       </c>
       <c r="G29" s="43">
-        <v>6990</v>
+        <v>1800</v>
       </c>
       <c r="H29" s="29">
         <f>F29*G29</f>
-        <v>6990</v>
+        <v>1800</v>
       </c>
       <c r="J29" s="30"/>
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
       <c r="M29" s="32"/>
       <c r="N29" s="32"/>
-      <c r="Q29" s="80"/>
+      <c r="Q29" s="61"/>
       <c r="R29" s="6"/>
       <c r="S29" s="7"/>
       <c r="T29" s="15"/>
@@ -1906,7 +1906,7 @@
       <c r="V29" s="9"/>
     </row>
     <row r="30" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D30" s="57"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="6" t="s">
         <v>23</v>
       </c>
@@ -1914,18 +1914,18 @@
         <v>1</v>
       </c>
       <c r="G30" s="15">
-        <v>9000</v>
+        <v>5000</v>
       </c>
       <c r="H30" s="29">
         <f t="shared" ref="H30:H35" si="3">F30*G30</f>
-        <v>9000</v>
+        <v>5000</v>
       </c>
       <c r="J30" s="30"/>
       <c r="K30" s="44"/>
       <c r="L30" s="44"/>
       <c r="M30" s="32"/>
       <c r="N30" s="32"/>
-      <c r="Q30" s="80"/>
+      <c r="Q30" s="61"/>
       <c r="R30" s="6"/>
       <c r="S30" s="7"/>
       <c r="T30" s="15"/>
@@ -1933,7 +1933,7 @@
       <c r="V30" s="9"/>
     </row>
     <row r="31" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D31" s="57"/>
+      <c r="D31" s="84"/>
       <c r="E31" s="6" t="s">
         <v>24</v>
       </c>
@@ -1950,7 +1950,7 @@
       <c r="L31" s="44"/>
       <c r="M31" s="32"/>
       <c r="N31" s="32"/>
-      <c r="Q31" s="80"/>
+      <c r="Q31" s="61"/>
       <c r="R31" s="6"/>
       <c r="S31" s="7"/>
       <c r="T31" s="15"/>
@@ -1958,7 +1958,7 @@
       <c r="V31" s="9"/>
     </row>
     <row r="32" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D32" s="57"/>
+      <c r="D32" s="84"/>
       <c r="E32" s="6" t="s">
         <v>25</v>
       </c>
@@ -1975,7 +1975,7 @@
       <c r="L32" s="44"/>
       <c r="M32" s="32"/>
       <c r="N32" s="32"/>
-      <c r="Q32" s="80"/>
+      <c r="Q32" s="61"/>
       <c r="R32" s="6"/>
       <c r="S32" s="7"/>
       <c r="T32" s="15"/>
@@ -1983,7 +1983,7 @@
       <c r="V32" s="9"/>
     </row>
     <row r="33" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D33" s="57"/>
+      <c r="D33" s="84"/>
       <c r="E33" s="6" t="s">
         <v>26</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="L33" s="44"/>
       <c r="M33" s="32"/>
       <c r="N33" s="32"/>
-      <c r="Q33" s="80"/>
+      <c r="Q33" s="61"/>
       <c r="R33" s="6"/>
       <c r="S33" s="7"/>
       <c r="T33" s="15"/>
@@ -2008,10 +2008,10 @@
       <c r="V33" s="9"/>
     </row>
     <row r="34" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="57"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="12" t="s">
         <v>27</v>
       </c>
@@ -2030,7 +2030,7 @@
       <c r="L34" s="44"/>
       <c r="M34" s="32"/>
       <c r="N34" s="32"/>
-      <c r="Q34" s="80"/>
+      <c r="Q34" s="61"/>
       <c r="R34" s="6"/>
       <c r="S34" s="7"/>
       <c r="T34" s="15"/>
@@ -2038,7 +2038,7 @@
       <c r="V34" s="9"/>
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D35" s="58"/>
+      <c r="D35" s="85"/>
       <c r="E35" s="6" t="s">
         <v>29</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="L35" s="44"/>
       <c r="M35" s="32"/>
       <c r="N35" s="32"/>
-      <c r="Q35" s="80"/>
+      <c r="Q35" s="61"/>
       <c r="R35" s="6"/>
       <c r="S35" s="7"/>
       <c r="T35" s="15"/>
@@ -2067,20 +2067,20 @@
     <row r="36" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D36" s="23"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="48" t="s">
+      <c r="F36" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="49"/>
+      <c r="G36" s="74"/>
       <c r="H36" s="22">
         <f>SUM(H29:H35)</f>
-        <v>22880</v>
+        <v>13690</v>
       </c>
       <c r="J36" s="30"/>
       <c r="K36" s="13"/>
       <c r="L36" s="44"/>
       <c r="M36" s="32"/>
       <c r="N36" s="32"/>
-      <c r="Q36" s="80"/>
+      <c r="Q36" s="61"/>
       <c r="R36" s="6"/>
       <c r="S36" s="7"/>
       <c r="T36" s="15"/>
@@ -2098,11 +2098,11 @@
       <c r="L37" s="31"/>
       <c r="M37" s="14"/>
       <c r="N37" s="32"/>
-      <c r="Q37" s="81"/>
+      <c r="Q37" s="62"/>
       <c r="R37" s="17"/>
-      <c r="S37" s="82"/>
-      <c r="T37" s="83"/>
-      <c r="U37" s="83"/>
+      <c r="S37" s="63"/>
+      <c r="T37" s="64"/>
+      <c r="U37" s="64"/>
       <c r="V37" s="19"/>
     </row>
     <row r="38" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2118,7 +2118,7 @@
       <c r="N38" s="32"/>
     </row>
     <row r="39" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D39" s="50" t="s">
+      <c r="D39" s="75" t="s">
         <v>37</v>
       </c>
       <c r="E39" s="11" t="s">
@@ -2141,7 +2141,7 @@
       <c r="N39" s="32"/>
     </row>
     <row r="40" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D40" s="51"/>
+      <c r="D40" s="76"/>
       <c r="E40" s="11" t="s">
         <v>32</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="N40" s="32"/>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D41" s="51"/>
+      <c r="D41" s="76"/>
       <c r="E41" s="11" t="s">
         <v>33</v>
       </c>
@@ -2183,7 +2183,7 @@
       <c r="N41" s="32"/>
     </row>
     <row r="42" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D42" s="51"/>
+      <c r="D42" s="76"/>
       <c r="E42" s="11" t="s">
         <v>34</v>
       </c>
@@ -2204,7 +2204,7 @@
       <c r="N42" s="32"/>
     </row>
     <row r="43" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D43" s="51"/>
+      <c r="D43" s="76"/>
       <c r="E43" s="11" t="s">
         <v>35</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="N43" s="32"/>
     </row>
     <row r="44" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="D44" s="52"/>
+      <c r="D44" s="77"/>
       <c r="E44" s="6" t="s">
         <v>36</v>
       </c>
@@ -2243,10 +2243,10 @@
     <row r="45" spans="3:22" x14ac:dyDescent="0.3">
       <c r="D45" s="3"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="48" t="s">
+      <c r="F45" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="49"/>
+      <c r="G45" s="74"/>
       <c r="H45" s="9">
         <f>SUM(H39:H44)</f>
         <v>2935</v>

</xml_diff>

<commit_message>
Changes: Huges changes are done to optimezed 2 design
</commit_message>
<xml_diff>
--- a/Cost/Multi Size opration.xlsx
+++ b/Cost/Multi Size opration.xlsx
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:Y135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,15 +1196,15 @@
         <v>17</v>
       </c>
       <c r="L7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="8">
         <f>H18</f>
-        <v>15200</v>
+        <v>21200</v>
       </c>
       <c r="N7" s="9">
         <f>L7*M7</f>
-        <v>30400</v>
+        <v>21200</v>
       </c>
       <c r="Q7" s="72">
         <v>44423</v>
@@ -1251,7 +1251,7 @@
         <v>21</v>
       </c>
       <c r="L8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="8">
         <f>H26</f>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="N8" s="9">
         <f>L8*M8</f>
-        <v>4720</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="72"/>
       <c r="R8" s="6" t="s">
@@ -1311,11 +1311,11 @@
       </c>
       <c r="M9" s="8">
         <f>H36</f>
-        <v>13690</v>
+        <v>12490</v>
       </c>
       <c r="N9" s="9">
         <f>L9*M9</f>
-        <v>13690</v>
+        <v>12490</v>
       </c>
       <c r="Q9" s="72"/>
       <c r="R9" s="6" t="s">
@@ -1467,11 +1467,11 @@
         <v>1</v>
       </c>
       <c r="G13" s="8">
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="J13" s="30"/>
       <c r="K13" s="52"/>
@@ -1481,7 +1481,7 @@
       <c r="M13" s="81"/>
       <c r="N13" s="53">
         <f>SUM(N7:N10)</f>
-        <v>51745</v>
+        <v>36625</v>
       </c>
       <c r="Q13" s="61"/>
       <c r="R13" s="6"/>
@@ -1516,7 +1516,7 @@
       <c r="M14" s="80"/>
       <c r="N14" s="55">
         <f>115000-N13</f>
-        <v>63255</v>
+        <v>78375</v>
       </c>
       <c r="Q14" s="61"/>
       <c r="R14" s="6"/>
@@ -1624,7 +1624,7 @@
       <c r="G18" s="74"/>
       <c r="H18" s="25">
         <f>SUM(H8:H17)</f>
-        <v>15200</v>
+        <v>21200</v>
       </c>
       <c r="J18" s="30"/>
       <c r="K18" s="13"/>
@@ -1887,11 +1887,11 @@
         <v>1</v>
       </c>
       <c r="G29" s="43">
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="H29" s="29">
         <f>F29*G29</f>
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="J29" s="30"/>
       <c r="K29" s="44"/>
@@ -2073,7 +2073,7 @@
       <c r="G36" s="74"/>
       <c r="H36" s="22">
         <f>SUM(H29:H35)</f>
-        <v>13690</v>
+        <v>12490</v>
       </c>
       <c r="J36" s="30"/>
       <c r="K36" s="13"/>

</xml_diff>